<commit_message>
Adding nuclue setup, updating vs project
</commit_message>
<xml_diff>
--- a/docs/mypinouts.xlsx
+++ b/docs/mypinouts.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="85">
   <si>
     <t>mems</t>
   </si>
@@ -202,6 +202,78 @@
   </si>
   <si>
     <t>2</t>
+  </si>
+  <si>
+    <t>NUCLEO</t>
+  </si>
+  <si>
+    <t>pf1</t>
+  </si>
+  <si>
+    <t>pf0</t>
+  </si>
+  <si>
+    <t>scription</t>
+  </si>
+  <si>
+    <t>i2c_2</t>
+  </si>
+  <si>
+    <t>CN9-19</t>
+  </si>
+  <si>
+    <t>CN9-21</t>
+  </si>
+  <si>
+    <t>Ina-2</t>
+  </si>
+  <si>
+    <t>Inb-2</t>
+  </si>
+  <si>
+    <t>PWM-2</t>
+  </si>
+  <si>
+    <t>PE4</t>
+  </si>
+  <si>
+    <t>PE5</t>
+  </si>
+  <si>
+    <t>PE6</t>
+  </si>
+  <si>
+    <t>PE3</t>
+  </si>
+  <si>
+    <t>CN9-16</t>
+  </si>
+  <si>
+    <t>CN9-18</t>
+  </si>
+  <si>
+    <t>CN9-20</t>
+  </si>
+  <si>
+    <t>CN9-22</t>
+  </si>
+  <si>
+    <t>CN10-32/</t>
+  </si>
+  <si>
+    <t>CN10-34/</t>
+  </si>
+  <si>
+    <t>PB10</t>
+  </si>
+  <si>
+    <t>PB11</t>
+  </si>
+  <si>
+    <t>TIM2_CH3</t>
+  </si>
+  <si>
+    <t>TIM2_CH4</t>
   </si>
 </sst>
 </file>
@@ -340,6 +412,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -375,6 +464,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -527,10 +633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -540,163 +646,184 @@
     <col min="3" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F2" s="1">
+      <c r="D1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H2" s="1">
         <v>76</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="1">
+      <c r="D3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H3" s="1">
         <v>81</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="D4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1">
         <v>3.3</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="1">
         <v>1101011</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="D11" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="J11" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="G12" s="2" t="s">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I12" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="J12" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
@@ -706,85 +833,148 @@
       <c r="C13" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="D13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I13" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="J13" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G14" s="1" t="s">
+      <c r="D14" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="J14" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G15" s="1" t="s">
+      <c r="D15" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I15" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="J15" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+      <c r="D19" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="I20" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="J20" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="I21" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="G19" s="1" t="s">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I22" s="1" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>